<commit_message>
Uso de Hojas en Excel
</commit_message>
<xml_diff>
--- a/Leccion01/IntroduccionExcel.xlsx
+++ b/Leccion01/IntroduccionExcel.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriano\Documents\universidad_excel-ua\Leccion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20F8DE2-042B-4523-B24B-236331CA46CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0B074-6EB5-4352-8287-7973E98F9339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{750359E0-C2EA-4452-9A84-CE21C30D4C85}"/>
+    <workbookView xWindow="1812" yWindow="1848" windowWidth="17280" windowHeight="8976" activeTab="2" xr2:uid="{750359E0-C2EA-4452-9A84-CE21C30D4C85}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="NuevaHoja" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,6 +33,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Hoja 1</t>
+  </si>
+  <si>
+    <t>Hoja 2</t>
+  </si>
+  <si>
+    <t>Hoja 3</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -389,10 +405,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148AB5E7-F71E-4C56-ABDB-9360CC5355E9}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,6 +419,50 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E161E125-964C-4904-9CF1-C1B38026E395}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A22C2A-FBD3-4E1C-AB05-6C7564BEFC55}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Celdas, Columnas y Filas en Excel
</commit_message>
<xml_diff>
--- a/Leccion01/IntroduccionExcel.xlsx
+++ b/Leccion01/IntroduccionExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriano\Documents\universidad_excel-ua\Leccion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0B074-6EB5-4352-8287-7973E98F9339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D2082A-7A7D-45C2-83A4-CEB81652E3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1848" windowWidth="17280" windowHeight="8976" activeTab="2" xr2:uid="{750359E0-C2EA-4452-9A84-CE21C30D4C85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{750359E0-C2EA-4452-9A84-CE21C30D4C85}"/>
   </bookViews>
   <sheets>
     <sheet name="NuevaHoja" sheetId="1" r:id="rId1"/>
@@ -38,19 +38,23 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Hoja 1</t>
-  </si>
-  <si>
     <t>Hoja 2</t>
   </si>
   <si>
     <t>Hoja 3</t>
   </si>
+  <si>
+    <t>Primer 
+Texto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,9 +92,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,20 +419,32 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C1" s="4">
+        <v>44562</v>
+      </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>0</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>2+3</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -442,7 +465,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -454,13 +477,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A22C2A-FBD3-4E1C-AB05-6C7564BEFC55}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manejo de Rangos en Excel
</commit_message>
<xml_diff>
--- a/Leccion01/IntroduccionExcel.xlsx
+++ b/Leccion01/IntroduccionExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriano\Documents\universidad_excel-ua\Leccion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D2082A-7A7D-45C2-83A4-CEB81652E3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD4F54F-AB35-4963-BDAC-D2D4B16809D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{750359E0-C2EA-4452-9A84-CE21C30D4C85}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="PrimerRango">NuevaHoja!$A$1:$C$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Hoja 2</t>
   </si>
@@ -47,13 +50,16 @@
     <t>Primer 
 Texto</t>
   </si>
+  <si>
+    <t>Segundo texto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -101,7 +107,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +425,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,6 +452,15 @@
         <f>2+3</f>
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>